<commit_message>
ajout d'un axe d'amélioration
</commit_message>
<xml_diff>
--- a/plan_de_tests_unitaires/plan-de-tests-unitaires.xlsx
+++ b/plan_de_tests_unitaires/plan-de-tests-unitaires.xlsx
@@ -100,7 +100,25 @@
     <t xml:space="preserve">l’api répond, la page affiche le produit concerné avec la photo, le prix, la description</t>
   </si>
   <si>
-    <t xml:space="preserve">l’api ne répond pas,il n’y pas de données sur le produit concerné</t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">l’api ne répond pas,il n’y pas de données sur le produit concerné, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF81D41A"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">axe d’amélioration : indiquer qu’il y a un problème avec le serveur</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">choisit la quantité</t>
@@ -248,7 +266,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -287,6 +305,13 @@
     </font>
     <font>
       <sz val="12"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF81D41A"/>
       <name val="Segoe UI"/>
       <family val="2"/>
       <charset val="1"/>
@@ -445,7 +470,7 @@
       <rgbColor rgb="FFFFD8CE"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FF81D41A"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
@@ -472,10 +497,10 @@
   <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.32"/>

</xml_diff>